<commit_message>
Add the excel also to hw2
</commit_message>
<xml_diff>
--- a/HW2/data_diggers_queries_results.xlsx
+++ b/HW2/data_diggers_queries_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avihayha\Downloads\HW2_datadiggers\DataDiggersHw2\HW2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\אחזור מידע\HW2\HW2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C3B1C0-E63E-46A6-AA69-DD973C3775AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528A225E-6C1E-41C4-BADB-03269F9DB25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26160" yWindow="-13620" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query 1 - All Details" sheetId="1" r:id="rId1"/>
@@ -677,7 +677,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -685,7 +685,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -698,7 +698,7 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -712,14 +712,14 @@
       <b/>
       <sz val="25"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -732,7 +732,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF212121"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -760,14 +760,14 @@
       <b/>
       <sz val="28"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1098,45 +1098,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1163,12 +1124,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{F4DFD62C-1410-48F0-9D01-BBC4906FC8A2}"/>
   </cellStyles>
   <dxfs count="79">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF212121"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1246,13 +1276,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -1262,6 +1285,13 @@
         <top style="thin">
           <color auto="1"/>
         </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
@@ -1344,13 +1374,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -1366,31 +1389,10 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
+      <border outline="0">
+        <bottom style="thin">
           <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1502,13 +1504,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -1524,17 +1519,15 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1544,14 +1537,21 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color rgb="FF212121"/>
+        <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1570,8 +1570,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1582,8 +1582,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1603,8 +1601,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1617,8 +1615,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1638,8 +1634,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1652,8 +1648,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1673,8 +1667,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1687,8 +1681,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1708,8 +1700,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1722,8 +1714,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1743,8 +1733,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1757,8 +1747,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1778,8 +1766,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1792,8 +1780,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1813,8 +1799,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1827,8 +1813,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1848,8 +1832,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1862,8 +1846,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1883,8 +1865,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1897,8 +1879,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1918,8 +1898,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1932,8 +1912,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1953,8 +1931,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -1967,8 +1945,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1988,8 +1964,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -2002,8 +1978,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2023,8 +1997,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -2037,8 +2011,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2058,8 +2030,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -2072,8 +2044,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2093,8 +2063,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -2107,8 +2077,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2128,8 +2096,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -2142,8 +2110,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2163,8 +2129,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -2177,8 +2143,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2198,8 +2162,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -2212,8 +2176,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2233,8 +2195,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -2247,8 +2209,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2268,8 +2228,8 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color rgb="FF000000"/>
         </left>
@@ -2282,8 +2242,6 @@
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2633,105 +2591,63 @@
     <tableColumn id="4" xr3:uid="{4C349302-D526-4397-87B6-02EB948BF641}" name="|DF|" dataDxfId="45" dataCellStyle="Normal 2">
       <calculatedColumnFormula>LOG10(C93)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{AF917A2D-ACBF-43D3-855A-ADEA6ED680D3}" name="Q" dataDxfId="44" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*B72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{5D15EC2C-773E-4883-891A-55720CAB60A5}" name="D1" dataDxfId="43" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*C72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{554AE614-ABD1-41B2-BC0E-B6319FCCF9C3}" name="D2" dataDxfId="42" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*D72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{8C6C424A-470A-4F2B-BDC7-7C8EF605A57F}" name="D3" dataDxfId="41" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*E72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{7BAF2AD5-6B3A-4992-AE00-745606D37BBF}" name="D4" dataDxfId="40" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*F72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="10" xr3:uid="{D71420AA-599E-442A-81A3-F49462A33A04}" name="D5" dataDxfId="39" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*G72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="11" xr3:uid="{EF86942C-D343-4208-AEA2-D7A8647F5FAD}" name="D6" dataDxfId="38" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*H72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="12" xr3:uid="{8112624F-B191-4C1E-BB63-13CECB153B02}" name="D7" dataDxfId="37" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*I72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="13" xr3:uid="{38A3BBAE-1ADF-4AB9-B6E4-7CAC9E7C984A}" name="D8" dataDxfId="36" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*J72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="14" xr3:uid="{7C56639E-F91D-46F9-9820-FD3366768BBF}" name="D9" dataDxfId="35" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*K72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="15" xr3:uid="{D4623CDE-9592-4545-9C2D-851A87763AF5}" name="D10" dataDxfId="34" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*L72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="16" xr3:uid="{11A2DAE1-C658-4057-86DB-E707A3264932}" name="D11" dataDxfId="33" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*M72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="17" xr3:uid="{93AA9306-ACC4-4D17-9299-23C608762311}" name="D12" dataDxfId="32" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*N72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="18" xr3:uid="{92543113-22E9-4B4A-AB6E-E2772099B5CD}" name="D13" dataDxfId="31" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*O72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="19" xr3:uid="{C30D22D6-F9DC-475F-B697-5B3D48A7F36B}" name="D14" dataDxfId="30" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*P72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="20" xr3:uid="{6E0FF3B6-291A-4E03-B2AB-8C2FFDF4AB4F}" name="D15" dataDxfId="29" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*Q72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="21" xr3:uid="{BC6ECD2B-9FA0-4ADA-9513-D4D94DB1A9F7}" name="D16" dataDxfId="28" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*R72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="22" xr3:uid="{4970984E-5E64-4AFE-84B8-1FBBF4FDC042}" name="D17" dataDxfId="27" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*S72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="23" xr3:uid="{C8F88738-5AF2-4D1B-B418-F81B8EA75579}" name="D18" dataDxfId="26" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*T72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="24" xr3:uid="{D90CEC3B-EF94-4466-868C-539DEC042F73}" name="D19" dataDxfId="25" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*U72</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="25" xr3:uid="{DC48E209-432E-49BC-9ACE-AB51A856CF61}" name="D20" dataDxfId="24" dataCellStyle="Normal 2">
-      <calculatedColumnFormula>0.8239*V72</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="5" xr3:uid="{AF917A2D-ACBF-43D3-855A-ADEA6ED680D3}" name="Q" dataDxfId="44" dataCellStyle="Normal 2"/>
+    <tableColumn id="6" xr3:uid="{5D15EC2C-773E-4883-891A-55720CAB60A5}" name="D1" dataDxfId="43" dataCellStyle="Normal 2"/>
+    <tableColumn id="7" xr3:uid="{554AE614-ABD1-41B2-BC0E-B6319FCCF9C3}" name="D2" dataDxfId="42" dataCellStyle="Normal 2"/>
+    <tableColumn id="8" xr3:uid="{8C6C424A-470A-4F2B-BDC7-7C8EF605A57F}" name="D3" dataDxfId="41" dataCellStyle="Normal 2"/>
+    <tableColumn id="9" xr3:uid="{7BAF2AD5-6B3A-4992-AE00-745606D37BBF}" name="D4" dataDxfId="40" dataCellStyle="Normal 2"/>
+    <tableColumn id="10" xr3:uid="{D71420AA-599E-442A-81A3-F49462A33A04}" name="D5" dataDxfId="39" dataCellStyle="Normal 2"/>
+    <tableColumn id="11" xr3:uid="{EF86942C-D343-4208-AEA2-D7A8647F5FAD}" name="D6" dataDxfId="38" dataCellStyle="Normal 2"/>
+    <tableColumn id="12" xr3:uid="{8112624F-B191-4C1E-BB63-13CECB153B02}" name="D7" dataDxfId="37" dataCellStyle="Normal 2"/>
+    <tableColumn id="13" xr3:uid="{38A3BBAE-1ADF-4AB9-B6E4-7CAC9E7C984A}" name="D8" dataDxfId="36" dataCellStyle="Normal 2"/>
+    <tableColumn id="14" xr3:uid="{7C56639E-F91D-46F9-9820-FD3366768BBF}" name="D9" dataDxfId="35" dataCellStyle="Normal 2"/>
+    <tableColumn id="15" xr3:uid="{D4623CDE-9592-4545-9C2D-851A87763AF5}" name="D10" dataDxfId="34" dataCellStyle="Normal 2"/>
+    <tableColumn id="16" xr3:uid="{11A2DAE1-C658-4057-86DB-E707A3264932}" name="D11" dataDxfId="33" dataCellStyle="Normal 2"/>
+    <tableColumn id="17" xr3:uid="{93AA9306-ACC4-4D17-9299-23C608762311}" name="D12" dataDxfId="32" dataCellStyle="Normal 2"/>
+    <tableColumn id="18" xr3:uid="{92543113-22E9-4B4A-AB6E-E2772099B5CD}" name="D13" dataDxfId="31" dataCellStyle="Normal 2"/>
+    <tableColumn id="19" xr3:uid="{C30D22D6-F9DC-475F-B697-5B3D48A7F36B}" name="D14" dataDxfId="30" dataCellStyle="Normal 2"/>
+    <tableColumn id="20" xr3:uid="{6E0FF3B6-291A-4E03-B2AB-8C2FFDF4AB4F}" name="D15" dataDxfId="29" dataCellStyle="Normal 2"/>
+    <tableColumn id="21" xr3:uid="{BC6ECD2B-9FA0-4ADA-9513-D4D94DB1A9F7}" name="D16" dataDxfId="28" dataCellStyle="Normal 2"/>
+    <tableColumn id="22" xr3:uid="{4970984E-5E64-4AFE-84B8-1FBBF4FDC042}" name="D17" dataDxfId="27" dataCellStyle="Normal 2"/>
+    <tableColumn id="23" xr3:uid="{C8F88738-5AF2-4D1B-B418-F81B8EA75579}" name="D18" dataDxfId="26" dataCellStyle="Normal 2"/>
+    <tableColumn id="24" xr3:uid="{D90CEC3B-EF94-4466-868C-539DEC042F73}" name="D19" dataDxfId="25" dataCellStyle="Normal 2"/>
+    <tableColumn id="25" xr3:uid="{DC48E209-432E-49BC-9ACE-AB51A856CF61}" name="D20" dataDxfId="24" dataCellStyle="Normal 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7569362E-5BE8-42CA-9DEB-40B280E02191}" name="Table2" displayName="Table2" ref="H122:J132" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7569362E-5BE8-42CA-9DEB-40B280E02191}" name="Table2" displayName="Table2" ref="H122:J132" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
   <autoFilter ref="H122:J132" xr:uid="{7569362E-5BE8-42CA-9DEB-40B280E02191}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{ABA96C35-54EB-432B-B11E-526319DB78F3}" name="Book name" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{AF2A89EF-E4E0-4821-821E-5381D664724D}" name="User 1" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{BEF4F4BE-F9CB-4ACC-9CBA-F1F3814F9044}" name="User 2" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{ABA96C35-54EB-432B-B11E-526319DB78F3}" name="Book name" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{AF2A89EF-E4E0-4821-821E-5381D664724D}" name="User 1" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{BEF4F4BE-F9CB-4ACC-9CBA-F1F3814F9044}" name="User 2" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{5EC75499-6A62-4D3F-8551-F64705DD5A05}" name="Table7" displayName="Table7" ref="F138:H140" totalsRowShown="0" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{5EC75499-6A62-4D3F-8551-F64705DD5A05}" name="Table7" displayName="Table7" ref="F138:H140" totalsRowShown="0" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="F138:H140" xr:uid="{5EC75499-6A62-4D3F-8551-F64705DD5A05}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{0DE99A19-49FE-40CC-9C3C-C739E0329F4F}" name="Column1" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{3676C062-956B-41D4-88C2-AE60E4F9574D}" name="Relevant" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{E7544C6A-8ACB-4A9A-95C7-8524582A72E8}" name="N-Relevant" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{0DE99A19-49FE-40CC-9C3C-C739E0329F4F}" name="Column1" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{3676C062-956B-41D4-88C2-AE60E4F9574D}" name="Relevant" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{E7544C6A-8ACB-4A9A-95C7-8524582A72E8}" name="N-Relevant" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D3F609A6-9BA2-4CB3-9CA4-9218F3C1AF50}" name="Table8" displayName="Table8" ref="F148:H150" totalsRowShown="0" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D3F609A6-9BA2-4CB3-9CA4-9218F3C1AF50}" name="Table8" displayName="Table8" ref="F148:H150" totalsRowShown="0" headerRowBorderDxfId="10" tableBorderDxfId="9" totalsRowBorderDxfId="8">
   <autoFilter ref="F148:H150" xr:uid="{D3F609A6-9BA2-4CB3-9CA4-9218F3C1AF50}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FCB263EC-792B-4A93-A0C9-6CE2910942DF}" name="Column1" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{32B7663E-D022-444B-9C85-F173DE282AD4}" name="Relevant" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{DFDAB20B-729A-4FE0-BAF5-05F7F69EAC5D}" name="N-Relevant" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{FCB263EC-792B-4A93-A0C9-6CE2910942DF}" name="Column1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{32B7663E-D022-444B-9C85-F173DE282AD4}" name="Relevant" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{DFDAB20B-729A-4FE0-BAF5-05F7F69EAC5D}" name="N-Relevant" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2741,19 +2657,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5E8728D5-D6EA-4FCD-9BB2-0B9A2F45AA4B}" name="Table5" displayName="Table5" ref="A13:B28" totalsRowShown="0">
   <autoFilter ref="A13:B28" xr:uid="{5E8728D5-D6EA-4FCD-9BB2-0B9A2F45AA4B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{723FDEB2-22AE-4FC3-B511-639BE76AE85F}" name="terms" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{6BC2845E-F36E-4516-8AA4-6FCAE4344F95}" name="docs" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{723FDEB2-22AE-4FC3-B511-639BE76AE85F}" name="terms" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{6BC2845E-F36E-4516-8AA4-6FCAE4344F95}" name="docs" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{536AD28F-95BB-4F51-B1EB-56C37C89A948}" name="Table6" displayName="Table6" ref="A14:B29" totalsRowShown="0" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{536AD28F-95BB-4F51-B1EB-56C37C89A948}" name="Table6" displayName="Table6" ref="A14:B29" totalsRowShown="0" dataDxfId="2">
   <autoFilter ref="A14:B29" xr:uid="{536AD28F-95BB-4F51-B1EB-56C37C89A948}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{AE1A438A-AD13-4502-AD5F-2374D424FAC2}" name="terms" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{C52C80F7-01F7-4806-AA4D-F50885B0BD18}" name="docs" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{AE1A438A-AD13-4502-AD5F-2374D424FAC2}" name="terms" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{C52C80F7-01F7-4806-AA4D-F50885B0BD18}" name="docs" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium28" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3048,22 +2964,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K144" sqref="K144"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I86" sqref="I86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.296875" customWidth="1"/>
+    <col min="2" max="2" width="13.296875" customWidth="1"/>
+    <col min="3" max="3" width="6.3984375" customWidth="1"/>
+    <col min="4" max="4" width="8.8984375" customWidth="1"/>
+    <col min="5" max="5" width="17.09765625" customWidth="1"/>
+    <col min="6" max="6" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.796875" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="9" width="11.69921875" customWidth="1"/>
+    <col min="10" max="10" width="10.296875" customWidth="1"/>
+    <col min="13" max="13" width="10.69921875" customWidth="1"/>
+    <col min="14" max="14" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5" customWidth="1"/>
+    <col min="16" max="16" width="11.8984375" customWidth="1"/>
+    <col min="17" max="17" width="11.796875" customWidth="1"/>
+    <col min="18" max="18" width="11.8984375" customWidth="1"/>
+    <col min="20" max="20" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.59765625" customWidth="1"/>
+    <col min="23" max="23" width="6.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" s="25" customFormat="1" x14ac:dyDescent="0.25">
@@ -3291,7 +3216,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="49" spans="1:22" ht="32.25" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:22" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="17" t="s">
         <v>117</v>
       </c>
@@ -3802,31 +3727,31 @@
       <c r="H68" s="2"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A69" s="37" t="s">
+    <row r="69" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="46" t="s">
         <v>181</v>
       </c>
-      <c r="B69" s="38"/>
-      <c r="C69" s="38"/>
-      <c r="D69" s="38"/>
-      <c r="E69" s="38"/>
-      <c r="F69" s="38"/>
-      <c r="G69" s="38"/>
-      <c r="H69" s="38"/>
-      <c r="I69" s="38"/>
-      <c r="J69" s="38"/>
-      <c r="K69" s="38"/>
-      <c r="L69" s="38"/>
-      <c r="M69" s="38"/>
-      <c r="N69" s="38"/>
-      <c r="O69" s="38"/>
-      <c r="P69" s="38"/>
-      <c r="Q69" s="38"/>
-      <c r="R69" s="38"/>
-      <c r="S69" s="38"/>
-      <c r="T69" s="38"/>
-      <c r="U69" s="38"/>
-      <c r="V69" s="39"/>
+      <c r="B69" s="47"/>
+      <c r="C69" s="47"/>
+      <c r="D69" s="47"/>
+      <c r="E69" s="47"/>
+      <c r="F69" s="47"/>
+      <c r="G69" s="47"/>
+      <c r="H69" s="47"/>
+      <c r="I69" s="47"/>
+      <c r="J69" s="47"/>
+      <c r="K69" s="47"/>
+      <c r="L69" s="47"/>
+      <c r="M69" s="47"/>
+      <c r="N69" s="47"/>
+      <c r="O69" s="47"/>
+      <c r="P69" s="47"/>
+      <c r="Q69" s="47"/>
+      <c r="R69" s="47"/>
+      <c r="S69" s="47"/>
+      <c r="T69" s="47"/>
+      <c r="U69" s="47"/>
+      <c r="V69" s="48"/>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" s="21" t="s">
@@ -3941,7 +3866,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G72" s="2">
         <v>0</v>
@@ -4944,7 +4869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:25" ht="18" x14ac:dyDescent="0.35">
       <c r="A90" s="17" t="s">
         <v>132</v>
       </c>
@@ -4973,34 +4898,34 @@
       <c r="X90" s="3"/>
       <c r="Y90" s="3"/>
     </row>
-    <row r="91" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:25" ht="18" x14ac:dyDescent="0.35">
       <c r="A91" s="18"/>
       <c r="B91" s="19"/>
       <c r="C91" s="20"/>
       <c r="D91" s="20"/>
-      <c r="E91" s="34" t="s">
+      <c r="E91" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="F91" s="35"/>
-      <c r="G91" s="35"/>
-      <c r="H91" s="35"/>
-      <c r="I91" s="35"/>
-      <c r="J91" s="35"/>
-      <c r="K91" s="35"/>
-      <c r="L91" s="35"/>
-      <c r="M91" s="35"/>
-      <c r="N91" s="35"/>
-      <c r="O91" s="35"/>
-      <c r="P91" s="35"/>
-      <c r="Q91" s="35"/>
-      <c r="R91" s="35"/>
-      <c r="S91" s="35"/>
-      <c r="T91" s="35"/>
-      <c r="U91" s="35"/>
-      <c r="V91" s="35"/>
-      <c r="W91" s="35"/>
-      <c r="X91" s="35"/>
-      <c r="Y91" s="36"/>
+      <c r="F91" s="55"/>
+      <c r="G91" s="55"/>
+      <c r="H91" s="55"/>
+      <c r="I91" s="55"/>
+      <c r="J91" s="55"/>
+      <c r="K91" s="55"/>
+      <c r="L91" s="55"/>
+      <c r="M91" s="55"/>
+      <c r="N91" s="55"/>
+      <c r="O91" s="55"/>
+      <c r="P91" s="55"/>
+      <c r="Q91" s="55"/>
+      <c r="R91" s="55"/>
+      <c r="S91" s="55"/>
+      <c r="T91" s="55"/>
+      <c r="U91" s="55"/>
+      <c r="V91" s="55"/>
+      <c r="W91" s="55"/>
+      <c r="X91" s="55"/>
+      <c r="Y91" s="56"/>
     </row>
     <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
@@ -5094,89 +5019,69 @@
         <f>LOG10(C93)</f>
         <v>0.6020599913279624</v>
       </c>
-      <c r="E93" s="10">
-        <f>0.602*B72</f>
-        <v>0</v>
-      </c>
-      <c r="F93" s="10">
-        <f>0.602*C72</f>
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="G93" s="10">
-        <f t="shared" ref="G93:Y95" si="0">0.602*D72</f>
-        <v>0</v>
-      </c>
-      <c r="H93" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I93" s="10">
-        <f t="shared" si="0"/>
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="J93" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K93" s="10">
-        <f t="shared" si="0"/>
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="L93" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M93" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N93" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O93" s="10">
-        <f t="shared" si="0"/>
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="P93" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q93" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R93" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S93" s="10">
-        <f t="shared" si="0"/>
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="T93" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U93" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V93" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W93" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="X93" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Y93" s="11">
-        <f t="shared" si="0"/>
-        <v>0.60199999999999998</v>
+      <c r="E93" s="2">
+        <f ca="1">D93*E93</f>
+        <v>0</v>
+      </c>
+      <c r="F93" s="11">
+        <v>0.60206000000000004</v>
+      </c>
+      <c r="G93" s="2">
+        <v>0</v>
+      </c>
+      <c r="H93" s="2">
+        <v>0</v>
+      </c>
+      <c r="I93" s="11">
+        <v>0</v>
+      </c>
+      <c r="J93" s="2">
+        <v>0</v>
+      </c>
+      <c r="K93" s="2">
+        <v>0.60206000000000004</v>
+      </c>
+      <c r="L93" s="2">
+        <v>0</v>
+      </c>
+      <c r="M93" s="2">
+        <v>0</v>
+      </c>
+      <c r="N93" s="2">
+        <v>0</v>
+      </c>
+      <c r="O93" s="2">
+        <v>0.60206000000000004</v>
+      </c>
+      <c r="P93" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q93" s="2">
+        <v>0</v>
+      </c>
+      <c r="R93" s="2">
+        <v>0</v>
+      </c>
+      <c r="S93" s="2">
+        <v>0.60206000000000004</v>
+      </c>
+      <c r="T93" s="2">
+        <v>0</v>
+      </c>
+      <c r="U93" s="2">
+        <v>0</v>
+      </c>
+      <c r="V93" s="2">
+        <v>0</v>
+      </c>
+      <c r="W93" s="2">
+        <v>0</v>
+      </c>
+      <c r="X93" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y93" s="2">
+        <v>0.60206000000000004</v>
       </c>
     </row>
     <row r="94" spans="1:25" x14ac:dyDescent="0.25">
@@ -5187,77 +5092,74 @@
         <v>5</v>
       </c>
       <c r="C94" s="10">
-        <f t="shared" ref="C94:C107" si="1">20/B94</f>
+        <f t="shared" ref="C94:C107" si="0">20/B94</f>
         <v>4</v>
       </c>
       <c r="D94" s="11">
-        <f t="shared" ref="D94:D107" si="2">LOG10(C94)</f>
+        <f t="shared" ref="D94:D107" si="1">LOG10(C94)</f>
         <v>0.6020599913279624</v>
       </c>
-      <c r="E94" s="10">
-        <f t="shared" ref="E94:F96" si="3">0.602*B73</f>
-        <v>0</v>
-      </c>
-      <c r="F94" s="10">
-        <f t="shared" si="3"/>
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="G94" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H94" s="10">
-        <v>0</v>
-      </c>
-      <c r="I94" s="10">
-        <v>0</v>
-      </c>
-      <c r="J94" s="10">
-        <v>0.25959387890000002</v>
-      </c>
-      <c r="K94" s="10">
-        <v>0</v>
-      </c>
-      <c r="L94" s="10">
-        <v>0</v>
-      </c>
-      <c r="M94" s="10">
-        <v>0</v>
-      </c>
-      <c r="N94" s="10">
-        <v>0.25959387890000002</v>
-      </c>
-      <c r="O94" s="10">
-        <v>0.25959387890000002</v>
-      </c>
-      <c r="P94" s="10">
-        <v>0.25959387890000002</v>
-      </c>
-      <c r="Q94" s="10">
-        <v>0</v>
-      </c>
-      <c r="R94" s="10">
-        <v>0.25959387890000002</v>
-      </c>
-      <c r="S94" s="10">
-        <v>0.25959387890000002</v>
-      </c>
-      <c r="T94" s="10">
-        <v>0.25959387890000002</v>
-      </c>
-      <c r="U94" s="10">
-        <v>0.25959387890000002</v>
-      </c>
-      <c r="V94" s="10">
-        <v>0.25959387890000002</v>
-      </c>
-      <c r="W94" s="10">
-        <v>0.25959387890000002</v>
-      </c>
-      <c r="X94" s="10">
-        <v>0.25959387890000002</v>
-      </c>
-      <c r="Y94" s="11">
+      <c r="E94" s="2">
+        <v>0</v>
+      </c>
+      <c r="F94" s="2">
+        <v>0.60206000000000004</v>
+      </c>
+      <c r="G94" s="2">
+        <v>0</v>
+      </c>
+      <c r="H94" s="2">
+        <v>0</v>
+      </c>
+      <c r="I94" s="2">
+        <v>0.60206000000000004</v>
+      </c>
+      <c r="J94" s="2">
+        <v>0</v>
+      </c>
+      <c r="K94" s="2">
+        <v>0</v>
+      </c>
+      <c r="L94" s="2">
+        <v>0</v>
+      </c>
+      <c r="M94" s="2">
+        <v>0</v>
+      </c>
+      <c r="N94" s="2">
+        <v>0</v>
+      </c>
+      <c r="O94" s="2">
+        <v>0.60206000000000004</v>
+      </c>
+      <c r="P94" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q94" s="2">
+        <v>0</v>
+      </c>
+      <c r="R94" s="2">
+        <v>0.60206000000000004</v>
+      </c>
+      <c r="S94" s="2">
+        <v>0.60206000000000004</v>
+      </c>
+      <c r="T94" s="2">
+        <v>0</v>
+      </c>
+      <c r="U94" s="2">
+        <v>0</v>
+      </c>
+      <c r="V94" s="2">
+        <v>0</v>
+      </c>
+      <c r="W94" s="2">
+        <v>0</v>
+      </c>
+      <c r="X94" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y94" s="2">
         <v>0</v>
       </c>
     </row>
@@ -5269,77 +5171,74 @@
         <v>5</v>
       </c>
       <c r="C95" s="10">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D95" s="11">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="D95" s="11">
-        <f t="shared" si="2"/>
         <v>0.6020599913279624</v>
       </c>
-      <c r="E95" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F95" s="10">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G95" s="10">
-        <f t="shared" si="0"/>
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="H95" s="10">
-        <v>0.22167499709999999</v>
-      </c>
-      <c r="I95" s="10">
-        <v>0.22167499709999999</v>
-      </c>
-      <c r="J95" s="10">
-        <v>0.22167499709999999</v>
-      </c>
-      <c r="K95" s="10">
-        <v>0</v>
-      </c>
-      <c r="L95" s="10">
-        <v>0.22167499709999999</v>
-      </c>
-      <c r="M95" s="10">
-        <v>0</v>
-      </c>
-      <c r="N95" s="10">
-        <v>0</v>
-      </c>
-      <c r="O95" s="10">
-        <v>0</v>
-      </c>
-      <c r="P95" s="10">
-        <v>0.22167499709999999</v>
-      </c>
-      <c r="Q95" s="10">
-        <v>0</v>
-      </c>
-      <c r="R95" s="10">
-        <v>0.22167499709999999</v>
-      </c>
-      <c r="S95" s="10">
-        <v>0.22167499709999999</v>
-      </c>
-      <c r="T95" s="10">
-        <v>0.22167499709999999</v>
-      </c>
-      <c r="U95" s="10">
-        <v>0.22167499709999999</v>
-      </c>
-      <c r="V95" s="10">
-        <v>0.22167499709999999</v>
-      </c>
-      <c r="W95" s="10">
-        <v>0.22167499709999999</v>
-      </c>
-      <c r="X95" s="10">
-        <v>0.22167499709999999</v>
-      </c>
-      <c r="Y95" s="11">
+      <c r="E95" s="2">
+        <v>0</v>
+      </c>
+      <c r="F95" s="2">
+        <v>0</v>
+      </c>
+      <c r="G95" s="2">
+        <v>0.60206000000000004</v>
+      </c>
+      <c r="H95" s="2">
+        <v>0</v>
+      </c>
+      <c r="I95" s="2">
+        <v>0.60206000000000004</v>
+      </c>
+      <c r="J95" s="2">
+        <v>0</v>
+      </c>
+      <c r="K95" s="2">
+        <v>0</v>
+      </c>
+      <c r="L95" s="2">
+        <v>0.60206000000000004</v>
+      </c>
+      <c r="M95" s="2">
+        <v>0</v>
+      </c>
+      <c r="N95" s="2">
+        <v>0</v>
+      </c>
+      <c r="O95" s="2">
+        <v>0</v>
+      </c>
+      <c r="P95" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q95" s="2">
+        <v>0</v>
+      </c>
+      <c r="R95" s="2">
+        <v>0</v>
+      </c>
+      <c r="S95" s="2">
+        <v>0</v>
+      </c>
+      <c r="T95" s="2">
+        <v>0</v>
+      </c>
+      <c r="U95" s="2">
+        <v>0</v>
+      </c>
+      <c r="V95" s="2">
+        <v>0.60206000000000004</v>
+      </c>
+      <c r="W95" s="2">
+        <v>0</v>
+      </c>
+      <c r="X95" s="2">
+        <v>0.60206000000000004</v>
+      </c>
+      <c r="Y95" s="2">
         <v>0</v>
       </c>
     </row>
@@ -5351,95 +5250,74 @@
         <v>4</v>
       </c>
       <c r="C96" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D96" s="11">
         <f>LOG10(C96)</f>
         <v>0.69897000433601886</v>
       </c>
-      <c r="E96" s="10">
-        <f t="shared" si="3"/>
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="F96" s="10">
-        <f t="shared" si="3"/>
-        <v>0.60199999999999998</v>
-      </c>
-      <c r="G96" s="10">
-        <f>0.6989*D75</f>
-        <v>0</v>
-      </c>
-      <c r="H96" s="10">
-        <f t="shared" ref="H96:Y96" si="4">0.6989*E75</f>
-        <v>0</v>
-      </c>
-      <c r="I96" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J96" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K96" s="10">
-        <f t="shared" si="4"/>
-        <v>0.69889999999999997</v>
-      </c>
-      <c r="L96" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M96" s="10">
-        <f t="shared" si="4"/>
-        <v>0.69889999999999997</v>
-      </c>
-      <c r="N96" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O96" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P96" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q96" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="R96" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="S96" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="T96" s="10">
-        <f t="shared" si="4"/>
-        <v>0.69889999999999997</v>
-      </c>
-      <c r="U96" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V96" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="W96" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="X96" s="10">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Y96" s="11">
-        <f t="shared" si="4"/>
+      <c r="E96" s="2">
+        <v>0.69896999999999998</v>
+      </c>
+      <c r="F96" s="2">
+        <v>0.69896999999999998</v>
+      </c>
+      <c r="G96" s="2">
+        <v>0</v>
+      </c>
+      <c r="H96" s="2">
+        <v>0</v>
+      </c>
+      <c r="I96" s="2">
+        <v>0</v>
+      </c>
+      <c r="J96" s="2">
+        <v>0</v>
+      </c>
+      <c r="K96" s="2">
+        <v>0.69896999999999998</v>
+      </c>
+      <c r="L96" s="2">
+        <v>0</v>
+      </c>
+      <c r="M96" s="2">
+        <v>0.69896999999999998</v>
+      </c>
+      <c r="N96" s="2">
+        <v>0</v>
+      </c>
+      <c r="O96" s="2">
+        <v>0</v>
+      </c>
+      <c r="P96" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q96" s="2">
+        <v>0</v>
+      </c>
+      <c r="R96" s="2">
+        <v>0</v>
+      </c>
+      <c r="S96" s="2">
+        <v>0</v>
+      </c>
+      <c r="T96" s="2">
+        <v>0.69896999999999998</v>
+      </c>
+      <c r="U96" s="2">
+        <v>0</v>
+      </c>
+      <c r="V96" s="2">
+        <v>0</v>
+      </c>
+      <c r="W96" s="2">
+        <v>0</v>
+      </c>
+      <c r="X96" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y96" s="2">
         <v>0</v>
       </c>
     </row>
@@ -5451,95 +5329,74 @@
         <v>3</v>
       </c>
       <c r="C97" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6.666666666666667</v>
       </c>
       <c r="D97" s="11">
-        <f t="shared" si="2"/>
+        <f>LOG10(C97)</f>
         <v>0.82390874094431876</v>
       </c>
-      <c r="E97" s="10">
-        <f>0.8239*B76</f>
-        <v>0</v>
-      </c>
-      <c r="F97" s="10">
-        <f>0.8239*C76</f>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="G97" s="10">
-        <f t="shared" ref="G97:Y107" si="5">0.8239*D76</f>
-        <v>0</v>
-      </c>
-      <c r="H97" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I97" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J97" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K97" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L97" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M97" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N97" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O97" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="P97" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q97" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="R97" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S97" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T97" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="U97" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="V97" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W97" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="X97" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Y97" s="11">
-        <f t="shared" si="5"/>
+      <c r="E97" s="2">
+        <v>0</v>
+      </c>
+      <c r="F97" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="G97" s="2">
+        <v>0</v>
+      </c>
+      <c r="H97" s="2">
+        <v>0</v>
+      </c>
+      <c r="I97" s="2">
+        <v>0</v>
+      </c>
+      <c r="J97" s="2">
+        <v>0</v>
+      </c>
+      <c r="K97" s="2">
+        <v>0</v>
+      </c>
+      <c r="L97" s="2">
+        <v>0</v>
+      </c>
+      <c r="M97" s="2">
+        <v>0</v>
+      </c>
+      <c r="N97" s="2">
+        <v>0</v>
+      </c>
+      <c r="O97" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="P97" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q97" s="2">
+        <v>0</v>
+      </c>
+      <c r="R97" s="2">
+        <v>0</v>
+      </c>
+      <c r="S97" s="2">
+        <v>0</v>
+      </c>
+      <c r="T97" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="U97" s="2">
+        <v>0</v>
+      </c>
+      <c r="V97" s="2">
+        <v>0</v>
+      </c>
+      <c r="W97" s="2">
+        <v>0</v>
+      </c>
+      <c r="X97" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y97" s="2">
         <v>0</v>
       </c>
     </row>
@@ -5551,95 +5408,74 @@
         <v>3</v>
       </c>
       <c r="C98" s="10">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="D98" s="11">
         <f t="shared" si="1"/>
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D98" s="11">
-        <f t="shared" si="2"/>
         <v>0.82390874094431876</v>
       </c>
-      <c r="E98" s="10">
-        <f t="shared" ref="E98:F107" si="6">0.8239*B77</f>
-        <v>0</v>
-      </c>
-      <c r="F98" s="10">
-        <f t="shared" si="6"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="G98" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H98" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I98" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J98" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K98" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L98" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M98" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N98" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O98" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P98" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="Q98" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="R98" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S98" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T98" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U98" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="V98" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W98" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="X98" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Y98" s="11">
-        <f t="shared" si="5"/>
+      <c r="E98" s="2">
+        <v>0</v>
+      </c>
+      <c r="F98" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="G98" s="2">
+        <v>0</v>
+      </c>
+      <c r="H98" s="2">
+        <v>0</v>
+      </c>
+      <c r="I98" s="2">
+        <v>0</v>
+      </c>
+      <c r="J98" s="2">
+        <v>0</v>
+      </c>
+      <c r="K98" s="2">
+        <v>0</v>
+      </c>
+      <c r="L98" s="2">
+        <v>0</v>
+      </c>
+      <c r="M98" s="2">
+        <v>0</v>
+      </c>
+      <c r="N98" s="2">
+        <v>0</v>
+      </c>
+      <c r="O98" s="2">
+        <v>0</v>
+      </c>
+      <c r="P98" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="Q98" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="R98" s="2">
+        <v>0</v>
+      </c>
+      <c r="S98" s="2">
+        <v>0</v>
+      </c>
+      <c r="T98" s="2">
+        <v>0</v>
+      </c>
+      <c r="U98" s="2">
+        <v>0</v>
+      </c>
+      <c r="V98" s="2">
+        <v>0</v>
+      </c>
+      <c r="W98" s="2">
+        <v>0</v>
+      </c>
+      <c r="X98" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y98" s="2">
         <v>0</v>
       </c>
     </row>
@@ -5651,95 +5487,74 @@
         <v>3</v>
       </c>
       <c r="C99" s="10">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="D99" s="11">
         <f t="shared" si="1"/>
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D99" s="11">
-        <f t="shared" si="2"/>
         <v>0.82390874094431876</v>
       </c>
-      <c r="E99" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F99" s="10">
-        <f t="shared" si="6"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="G99" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H99" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I99" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J99" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="K99" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L99" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M99" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="N99" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O99" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P99" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q99" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="R99" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S99" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T99" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U99" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="V99" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W99" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="X99" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Y99" s="11">
-        <f t="shared" si="5"/>
+      <c r="E99" s="2">
+        <v>0</v>
+      </c>
+      <c r="F99" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="G99" s="2">
+        <v>0</v>
+      </c>
+      <c r="H99" s="2">
+        <v>0</v>
+      </c>
+      <c r="I99" s="2">
+        <v>0</v>
+      </c>
+      <c r="J99" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="K99" s="2">
+        <v>0</v>
+      </c>
+      <c r="L99" s="2">
+        <v>0</v>
+      </c>
+      <c r="M99" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="N99" s="2">
+        <v>0</v>
+      </c>
+      <c r="O99" s="2">
+        <v>0</v>
+      </c>
+      <c r="P99" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q99" s="2">
+        <v>0</v>
+      </c>
+      <c r="R99" s="2">
+        <v>0</v>
+      </c>
+      <c r="S99" s="2">
+        <v>0</v>
+      </c>
+      <c r="T99" s="2">
+        <v>0</v>
+      </c>
+      <c r="U99" s="2">
+        <v>0</v>
+      </c>
+      <c r="V99" s="2">
+        <v>0</v>
+      </c>
+      <c r="W99" s="2">
+        <v>0</v>
+      </c>
+      <c r="X99" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y99" s="2">
         <v>0</v>
       </c>
     </row>
@@ -5751,95 +5566,74 @@
         <v>3</v>
       </c>
       <c r="C100" s="10">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="D100" s="11">
         <f t="shared" si="1"/>
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D100" s="11">
-        <f t="shared" si="2"/>
         <v>0.82390874094431876</v>
       </c>
-      <c r="E100" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F100" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G100" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H100" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I100" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="J100" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K100" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="L100" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="M100" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N100" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O100" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P100" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q100" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="R100" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S100" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T100" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U100" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="V100" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W100" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="X100" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Y100" s="11">
-        <f t="shared" si="5"/>
+      <c r="E100" s="2">
+        <v>0</v>
+      </c>
+      <c r="F100" s="2">
+        <v>0</v>
+      </c>
+      <c r="G100" s="2">
+        <v>0</v>
+      </c>
+      <c r="H100" s="2">
+        <v>0</v>
+      </c>
+      <c r="I100" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="J100" s="2">
+        <v>0</v>
+      </c>
+      <c r="K100" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="L100" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="M100" s="2">
+        <v>0</v>
+      </c>
+      <c r="N100" s="2">
+        <v>0</v>
+      </c>
+      <c r="O100" s="2">
+        <v>0</v>
+      </c>
+      <c r="P100" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q100" s="2">
+        <v>0</v>
+      </c>
+      <c r="R100" s="2">
+        <v>0</v>
+      </c>
+      <c r="S100" s="2">
+        <v>0</v>
+      </c>
+      <c r="T100" s="2">
+        <v>0</v>
+      </c>
+      <c r="U100" s="2">
+        <v>0</v>
+      </c>
+      <c r="V100" s="2">
+        <v>0</v>
+      </c>
+      <c r="W100" s="2">
+        <v>0</v>
+      </c>
+      <c r="X100" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y100" s="2">
         <v>0</v>
       </c>
     </row>
@@ -5851,95 +5645,74 @@
         <v>3</v>
       </c>
       <c r="C101" s="10">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="D101" s="11">
         <f t="shared" si="1"/>
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D101" s="11">
-        <f t="shared" si="2"/>
         <v>0.82390874094431876</v>
       </c>
-      <c r="E101" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F101" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G101" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H101" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I101" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="J101" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K101" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L101" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M101" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="N101" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O101" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P101" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q101" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="R101" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S101" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="T101" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U101" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="V101" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W101" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="X101" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Y101" s="11">
-        <f t="shared" si="5"/>
+      <c r="E101" s="2">
+        <v>0</v>
+      </c>
+      <c r="F101" s="2">
+        <v>0</v>
+      </c>
+      <c r="G101" s="2">
+        <v>0</v>
+      </c>
+      <c r="H101" s="2">
+        <v>0</v>
+      </c>
+      <c r="I101" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="J101" s="2">
+        <v>0</v>
+      </c>
+      <c r="K101" s="2">
+        <v>0</v>
+      </c>
+      <c r="L101" s="2">
+        <v>0</v>
+      </c>
+      <c r="M101" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="N101" s="2">
+        <v>0</v>
+      </c>
+      <c r="O101" s="2">
+        <v>0</v>
+      </c>
+      <c r="P101" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q101" s="2">
+        <v>0</v>
+      </c>
+      <c r="R101" s="2">
+        <v>0</v>
+      </c>
+      <c r="S101" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="T101" s="2">
+        <v>0</v>
+      </c>
+      <c r="U101" s="2">
+        <v>0</v>
+      </c>
+      <c r="V101" s="2">
+        <v>0</v>
+      </c>
+      <c r="W101" s="2">
+        <v>0</v>
+      </c>
+      <c r="X101" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y101" s="2">
         <v>0</v>
       </c>
     </row>
@@ -5951,96 +5724,75 @@
         <v>3</v>
       </c>
       <c r="C102" s="10">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="D102" s="11">
         <f t="shared" si="1"/>
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D102" s="11">
-        <f t="shared" si="2"/>
         <v>0.82390874094431876</v>
       </c>
-      <c r="E102" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F102" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G102" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H102" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I102" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J102" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="K102" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L102" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M102" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N102" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="O102" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P102" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q102" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="R102" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S102" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T102" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U102" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="V102" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W102" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="X102" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Y102" s="11">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
+      <c r="E102" s="2">
+        <v>0</v>
+      </c>
+      <c r="F102" s="2">
+        <v>0</v>
+      </c>
+      <c r="G102" s="2">
+        <v>0</v>
+      </c>
+      <c r="H102" s="2">
+        <v>0</v>
+      </c>
+      <c r="I102" s="2">
+        <v>0</v>
+      </c>
+      <c r="J102" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="K102" s="2">
+        <v>0</v>
+      </c>
+      <c r="L102" s="2">
+        <v>0</v>
+      </c>
+      <c r="M102" s="2">
+        <v>0</v>
+      </c>
+      <c r="N102" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="O102" s="2">
+        <v>0</v>
+      </c>
+      <c r="P102" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q102" s="2">
+        <v>0</v>
+      </c>
+      <c r="R102" s="2">
+        <v>0</v>
+      </c>
+      <c r="S102" s="2">
+        <v>0</v>
+      </c>
+      <c r="T102" s="2">
+        <v>0</v>
+      </c>
+      <c r="U102" s="2">
+        <v>0</v>
+      </c>
+      <c r="V102" s="2">
+        <v>0</v>
+      </c>
+      <c r="W102" s="2">
+        <v>0</v>
+      </c>
+      <c r="X102" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y102" s="2">
+        <v>0.82390870000000005</v>
       </c>
     </row>
     <row r="103" spans="1:25" x14ac:dyDescent="0.25">
@@ -6051,95 +5803,74 @@
         <v>3</v>
       </c>
       <c r="C103" s="10">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="D103" s="11">
         <f t="shared" si="1"/>
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D103" s="11">
-        <f t="shared" si="2"/>
         <v>0.82390874094431876</v>
       </c>
-      <c r="E103" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F103" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G103" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H103" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I103" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J103" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K103" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L103" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="M103" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N103" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O103" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="P103" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q103" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="R103" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S103" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T103" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U103" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="V103" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="W103" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="X103" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Y103" s="11">
-        <f t="shared" si="5"/>
+      <c r="E103" s="2">
+        <v>0</v>
+      </c>
+      <c r="F103" s="2">
+        <v>0</v>
+      </c>
+      <c r="G103" s="2">
+        <v>0</v>
+      </c>
+      <c r="H103" s="2">
+        <v>0</v>
+      </c>
+      <c r="I103" s="2">
+        <v>0</v>
+      </c>
+      <c r="J103" s="2">
+        <v>0</v>
+      </c>
+      <c r="K103" s="2">
+        <v>0</v>
+      </c>
+      <c r="L103" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="M103" s="2">
+        <v>0</v>
+      </c>
+      <c r="N103" s="2">
+        <v>0</v>
+      </c>
+      <c r="O103" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="P103" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q103" s="2">
+        <v>0</v>
+      </c>
+      <c r="R103" s="2">
+        <v>0</v>
+      </c>
+      <c r="S103" s="2">
+        <v>0</v>
+      </c>
+      <c r="T103" s="2">
+        <v>0</v>
+      </c>
+      <c r="U103" s="2">
+        <v>0</v>
+      </c>
+      <c r="V103" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="W103" s="2">
+        <v>0</v>
+      </c>
+      <c r="X103" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y103" s="2">
         <v>0</v>
       </c>
     </row>
@@ -6151,95 +5882,74 @@
         <v>3</v>
       </c>
       <c r="C104" s="10">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="D104" s="11">
         <f t="shared" si="1"/>
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D104" s="11">
-        <f t="shared" si="2"/>
         <v>0.82390874094431876</v>
       </c>
-      <c r="E104" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F104" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G104" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H104" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I104" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J104" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K104" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L104" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M104" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="N104" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O104" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P104" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q104" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="R104" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="S104" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T104" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U104" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="V104" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W104" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="X104" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Y104" s="11">
-        <f t="shared" si="5"/>
+      <c r="E104" s="2">
+        <v>0</v>
+      </c>
+      <c r="F104" s="2">
+        <v>0</v>
+      </c>
+      <c r="G104" s="2">
+        <v>0</v>
+      </c>
+      <c r="H104" s="2">
+        <v>0</v>
+      </c>
+      <c r="I104" s="2">
+        <v>0</v>
+      </c>
+      <c r="J104" s="2">
+        <v>0</v>
+      </c>
+      <c r="K104" s="2">
+        <v>0</v>
+      </c>
+      <c r="L104" s="2">
+        <v>0</v>
+      </c>
+      <c r="M104" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="N104" s="2">
+        <v>0</v>
+      </c>
+      <c r="O104" s="2">
+        <v>0</v>
+      </c>
+      <c r="P104" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q104" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="R104" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="S104" s="2">
+        <v>0</v>
+      </c>
+      <c r="T104" s="2">
+        <v>0</v>
+      </c>
+      <c r="U104" s="2">
+        <v>0</v>
+      </c>
+      <c r="V104" s="2">
+        <v>0</v>
+      </c>
+      <c r="W104" s="2">
+        <v>0</v>
+      </c>
+      <c r="X104" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y104" s="2">
         <v>0</v>
       </c>
     </row>
@@ -6251,95 +5961,74 @@
         <v>3</v>
       </c>
       <c r="C105" s="10">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="D105" s="11">
         <f t="shared" si="1"/>
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D105" s="11">
-        <f t="shared" si="2"/>
         <v>0.82390874094431876</v>
       </c>
-      <c r="E105" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F105" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G105" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H105" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I105" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J105" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K105" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L105" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M105" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="N105" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O105" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P105" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q105" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="R105" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="S105" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T105" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U105" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="V105" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W105" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="X105" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Y105" s="11">
-        <f t="shared" si="5"/>
+      <c r="E105" s="2">
+        <v>0</v>
+      </c>
+      <c r="F105" s="2">
+        <v>0</v>
+      </c>
+      <c r="G105" s="2">
+        <v>0</v>
+      </c>
+      <c r="H105" s="2">
+        <v>0</v>
+      </c>
+      <c r="I105" s="2">
+        <v>0</v>
+      </c>
+      <c r="J105" s="2">
+        <v>0</v>
+      </c>
+      <c r="K105" s="2">
+        <v>0</v>
+      </c>
+      <c r="L105" s="2">
+        <v>0</v>
+      </c>
+      <c r="M105" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="N105" s="2">
+        <v>0</v>
+      </c>
+      <c r="O105" s="2">
+        <v>0</v>
+      </c>
+      <c r="P105" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q105" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="R105" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="S105" s="2">
+        <v>0</v>
+      </c>
+      <c r="T105" s="2">
+        <v>0</v>
+      </c>
+      <c r="U105" s="2">
+        <v>0</v>
+      </c>
+      <c r="V105" s="2">
+        <v>0</v>
+      </c>
+      <c r="W105" s="2">
+        <v>0</v>
+      </c>
+      <c r="X105" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y105" s="2">
         <v>0</v>
       </c>
     </row>
@@ -6351,96 +6040,75 @@
         <v>3</v>
       </c>
       <c r="C106" s="10">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="D106" s="11">
         <f t="shared" si="1"/>
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D106" s="11">
-        <f t="shared" si="2"/>
         <v>0.82390874094431876</v>
       </c>
-      <c r="E106" s="10">
-        <f t="shared" si="6"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="F106" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G106" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H106" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I106" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J106" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K106" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L106" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M106" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="N106" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O106" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P106" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q106" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="R106" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="S106" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T106" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U106" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="V106" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W106" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="X106" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Y106" s="11">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
+      <c r="E106" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="F106" s="2">
+        <v>0</v>
+      </c>
+      <c r="G106" s="2">
+        <v>0</v>
+      </c>
+      <c r="H106" s="2">
+        <v>0</v>
+      </c>
+      <c r="I106" s="2">
+        <v>0</v>
+      </c>
+      <c r="J106" s="2">
+        <v>0</v>
+      </c>
+      <c r="K106" s="2">
+        <v>0</v>
+      </c>
+      <c r="L106" s="2">
+        <v>0</v>
+      </c>
+      <c r="M106" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="N106" s="2">
+        <v>0</v>
+      </c>
+      <c r="O106" s="2">
+        <v>0</v>
+      </c>
+      <c r="P106" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q106" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="R106" s="2">
+        <v>0</v>
+      </c>
+      <c r="S106" s="2">
+        <v>0</v>
+      </c>
+      <c r="T106" s="2">
+        <v>0</v>
+      </c>
+      <c r="U106" s="2">
+        <v>0</v>
+      </c>
+      <c r="V106" s="2">
+        <v>0</v>
+      </c>
+      <c r="W106" s="2">
+        <v>0</v>
+      </c>
+      <c r="X106" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y106" s="2">
+        <v>0.82390870000000005</v>
       </c>
     </row>
     <row r="107" spans="1:25" x14ac:dyDescent="0.25">
@@ -6451,170 +6119,149 @@
         <v>3</v>
       </c>
       <c r="C107" s="10">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="D107" s="11">
         <f t="shared" si="1"/>
-        <v>6.666666666666667</v>
-      </c>
-      <c r="D107" s="11">
-        <f t="shared" si="2"/>
         <v>0.82390874094431876</v>
       </c>
-      <c r="E107" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F107" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G107" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H107" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I107" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="J107" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K107" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="L107" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="M107" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="N107" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="O107" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="P107" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Q107" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="R107" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="S107" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="T107" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="U107" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="V107" s="10">
-        <f t="shared" si="5"/>
-        <v>0.82389999999999997</v>
-      </c>
-      <c r="W107" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="X107" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Y107" s="11">
-        <f t="shared" si="5"/>
+      <c r="E107" s="2">
+        <v>0</v>
+      </c>
+      <c r="F107" s="2">
+        <v>0</v>
+      </c>
+      <c r="G107" s="2">
+        <v>0</v>
+      </c>
+      <c r="H107" s="2">
+        <v>0</v>
+      </c>
+      <c r="I107" s="2">
+        <v>0</v>
+      </c>
+      <c r="J107" s="2">
+        <v>0</v>
+      </c>
+      <c r="K107" s="2">
+        <v>0</v>
+      </c>
+      <c r="L107" s="2">
+        <v>0</v>
+      </c>
+      <c r="M107" s="2">
+        <v>0</v>
+      </c>
+      <c r="N107" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="O107" s="2">
+        <v>0</v>
+      </c>
+      <c r="P107" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q107" s="2">
+        <v>0</v>
+      </c>
+      <c r="R107" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="S107" s="2">
+        <v>0</v>
+      </c>
+      <c r="T107" s="2">
+        <v>0</v>
+      </c>
+      <c r="U107" s="2">
+        <v>0</v>
+      </c>
+      <c r="V107" s="2">
+        <v>0.82390870000000005</v>
+      </c>
+      <c r="W107" s="2">
+        <v>0</v>
+      </c>
+      <c r="X107" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y107" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="F111" s="40" t="s">
+      <c r="F111" s="49" t="s">
         <v>182</v>
       </c>
-      <c r="G111" s="40"/>
-      <c r="H111" s="40"/>
-      <c r="I111" s="40"/>
-      <c r="J111" s="40"/>
-      <c r="K111" s="40"/>
-      <c r="L111" s="40"/>
-      <c r="M111" s="40"/>
-      <c r="N111" s="40"/>
-      <c r="O111" s="40"/>
-      <c r="P111" s="40"/>
-      <c r="Q111" s="40"/>
+      <c r="G111" s="49"/>
+      <c r="H111" s="49"/>
+      <c r="I111" s="49"/>
+      <c r="J111" s="49"/>
+      <c r="K111" s="49"/>
+      <c r="L111" s="49"/>
+      <c r="M111" s="49"/>
+      <c r="N111" s="49"/>
+      <c r="O111" s="49"/>
+      <c r="P111" s="49"/>
+      <c r="Q111" s="49"/>
     </row>
     <row r="112" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="F112" s="40"/>
-      <c r="G112" s="40"/>
-      <c r="H112" s="40"/>
-      <c r="I112" s="40"/>
-      <c r="J112" s="40"/>
-      <c r="K112" s="40"/>
-      <c r="L112" s="40"/>
-      <c r="M112" s="40"/>
-      <c r="N112" s="40"/>
-      <c r="O112" s="40"/>
-      <c r="P112" s="40"/>
-      <c r="Q112" s="40"/>
+      <c r="F112" s="49"/>
+      <c r="G112" s="49"/>
+      <c r="H112" s="49"/>
+      <c r="I112" s="49"/>
+      <c r="J112" s="49"/>
+      <c r="K112" s="49"/>
+      <c r="L112" s="49"/>
+      <c r="M112" s="49"/>
+      <c r="N112" s="49"/>
+      <c r="O112" s="49"/>
+      <c r="P112" s="49"/>
+      <c r="Q112" s="49"/>
     </row>
     <row r="113" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="F113" s="40"/>
-      <c r="G113" s="40"/>
-      <c r="H113" s="40"/>
-      <c r="I113" s="40"/>
-      <c r="J113" s="40"/>
-      <c r="K113" s="40"/>
-      <c r="L113" s="40"/>
-      <c r="M113" s="40"/>
-      <c r="N113" s="40"/>
-      <c r="O113" s="40"/>
-      <c r="P113" s="40"/>
-      <c r="Q113" s="40"/>
-    </row>
-    <row r="116" spans="5:17" ht="11.45" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="F113" s="49"/>
+      <c r="G113" s="49"/>
+      <c r="H113" s="49"/>
+      <c r="I113" s="49"/>
+      <c r="J113" s="49"/>
+      <c r="K113" s="49"/>
+      <c r="L113" s="49"/>
+      <c r="M113" s="49"/>
+      <c r="N113" s="49"/>
+      <c r="O113" s="49"/>
+      <c r="P113" s="49"/>
+      <c r="Q113" s="49"/>
+    </row>
+    <row r="116" spans="5:17" ht="11.4" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="117" spans="5:17" hidden="1" x14ac:dyDescent="0.25">
-      <c r="E117" s="41" t="s">
+      <c r="E117" s="50" t="s">
         <v>184</v>
       </c>
-      <c r="F117" s="42"/>
-      <c r="G117" s="42"/>
-      <c r="H117" s="42"/>
-      <c r="I117" s="42"/>
-      <c r="J117" s="42"/>
-      <c r="K117" s="42"/>
-      <c r="L117" s="42"/>
-      <c r="M117" s="42"/>
-      <c r="N117" s="42"/>
+      <c r="F117" s="51"/>
+      <c r="G117" s="51"/>
+      <c r="H117" s="51"/>
+      <c r="I117" s="51"/>
+      <c r="J117" s="51"/>
+      <c r="K117" s="51"/>
+      <c r="L117" s="51"/>
+      <c r="M117" s="51"/>
+      <c r="N117" s="51"/>
     </row>
     <row r="118" spans="5:17" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E118" s="42"/>
-      <c r="F118" s="42"/>
-      <c r="G118" s="42"/>
-      <c r="H118" s="42"/>
-      <c r="I118" s="42"/>
-      <c r="J118" s="42"/>
-      <c r="K118" s="42"/>
-      <c r="L118" s="42"/>
-      <c r="M118" s="42"/>
-      <c r="N118" s="42"/>
-    </row>
-    <row r="119" spans="5:17" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="E118" s="51"/>
+      <c r="F118" s="51"/>
+      <c r="G118" s="51"/>
+      <c r="H118" s="51"/>
+      <c r="I118" s="51"/>
+      <c r="J118" s="51"/>
+      <c r="K118" s="51"/>
+      <c r="L118" s="51"/>
+      <c r="M118" s="51"/>
+      <c r="N118" s="51"/>
+    </row>
+    <row r="119" spans="5:17" ht="16.8" x14ac:dyDescent="0.4">
       <c r="H119" s="12" t="s">
         <v>204</v>
       </c>
@@ -6623,127 +6270,127 @@
       </c>
     </row>
     <row r="122" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="H122" s="49" t="s">
+      <c r="H122" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="I122" s="50" t="s">
+      <c r="I122" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="J122" s="51" t="s">
+      <c r="J122" s="38" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="123" spans="5:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="H123" s="46" t="s">
+    <row r="123" spans="5:17" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="H123" s="33" t="s">
         <v>194</v>
       </c>
       <c r="I123" s="29">
         <v>1</v>
       </c>
-      <c r="J123" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="5:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="H124" s="46" t="s">
+      <c r="J123" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="5:17" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="H124" s="33" t="s">
         <v>195</v>
       </c>
       <c r="I124" s="28">
         <v>0</v>
       </c>
-      <c r="J124" s="48">
+      <c r="J124" s="35">
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="5:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="H125" s="46" t="s">
+    <row r="125" spans="5:17" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="H125" s="33" t="s">
         <v>196</v>
       </c>
       <c r="I125" s="28">
         <v>0</v>
       </c>
-      <c r="J125" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="5:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="H126" s="46" t="s">
+      <c r="J125" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="5:17" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="H126" s="33" t="s">
         <v>197</v>
       </c>
       <c r="I126" s="29">
         <v>1</v>
       </c>
-      <c r="J126" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="5:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="H127" s="46" t="s">
+      <c r="J126" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="5:17" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="H127" s="33" t="s">
         <v>198</v>
       </c>
       <c r="I127" s="29">
         <v>1</v>
       </c>
-      <c r="J127" s="48">
+      <c r="J127" s="35">
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="5:17" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="H128" s="46" t="s">
+    <row r="128" spans="5:17" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="H128" s="33" t="s">
         <v>199</v>
       </c>
       <c r="I128" s="29">
         <v>1</v>
       </c>
-      <c r="J128" s="47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="H129" s="46" t="s">
+      <c r="J128" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="2:11" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="H129" s="33" t="s">
         <v>46</v>
       </c>
       <c r="I129" s="29">
         <v>1</v>
       </c>
-      <c r="J129" s="48">
+      <c r="J129" s="35">
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="H130" s="46" t="s">
+    <row r="130" spans="2:11" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="H130" s="33" t="s">
         <v>200</v>
       </c>
       <c r="I130" s="28">
         <v>0</v>
       </c>
-      <c r="J130" s="48">
+      <c r="J130" s="35">
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="H131" s="46" t="s">
+    <row r="131" spans="2:11" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="H131" s="33" t="s">
         <v>201</v>
       </c>
       <c r="I131" s="28">
         <v>0</v>
       </c>
-      <c r="J131" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="H132" s="52" t="s">
+      <c r="J131" s="35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="2:11" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="H132" s="39" t="s">
         <v>202</v>
       </c>
-      <c r="I132" s="53">
-        <v>0</v>
-      </c>
-      <c r="J132" s="54">
+      <c r="I132" s="40">
+        <v>0</v>
+      </c>
+      <c r="J132" s="41">
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:11" ht="16.8" x14ac:dyDescent="0.4">
       <c r="G134" s="12" t="s">
         <v>204</v>
       </c>
@@ -6752,180 +6399,180 @@
       </c>
     </row>
     <row r="135" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B135" s="33" t="s">
+      <c r="B135" s="53" t="s">
         <v>192</v>
       </c>
-      <c r="C135" s="33"/>
-      <c r="D135" s="33"/>
-      <c r="E135" s="33"/>
-      <c r="F135" s="33"/>
-      <c r="G135" s="33"/>
-      <c r="H135" s="33"/>
-      <c r="I135" s="33"/>
-      <c r="J135" s="33"/>
-      <c r="K135" s="33"/>
+      <c r="C135" s="53"/>
+      <c r="D135" s="53"/>
+      <c r="E135" s="53"/>
+      <c r="F135" s="53"/>
+      <c r="G135" s="53"/>
+      <c r="H135" s="53"/>
+      <c r="I135" s="53"/>
+      <c r="J135" s="53"/>
+      <c r="K135" s="53"/>
     </row>
     <row r="136" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B136" s="33"/>
-      <c r="C136" s="33"/>
-      <c r="D136" s="33"/>
-      <c r="E136" s="33"/>
-      <c r="F136" s="33"/>
-      <c r="G136" s="33"/>
-      <c r="H136" s="33"/>
-      <c r="I136" s="33"/>
-      <c r="J136" s="33"/>
-      <c r="K136" s="33"/>
+      <c r="B136" s="53"/>
+      <c r="C136" s="53"/>
+      <c r="D136" s="53"/>
+      <c r="E136" s="53"/>
+      <c r="F136" s="53"/>
+      <c r="G136" s="53"/>
+      <c r="H136" s="53"/>
+      <c r="I136" s="53"/>
+      <c r="J136" s="53"/>
+      <c r="K136" s="53"/>
     </row>
     <row r="137" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B137" s="33"/>
-      <c r="C137" s="33"/>
-      <c r="D137" s="33"/>
-      <c r="E137" s="33"/>
-      <c r="F137" s="33"/>
-      <c r="G137" s="33"/>
-      <c r="H137" s="33"/>
-      <c r="I137" s="33"/>
-      <c r="J137" s="33"/>
-      <c r="K137" s="33"/>
+      <c r="B137" s="53"/>
+      <c r="C137" s="53"/>
+      <c r="D137" s="53"/>
+      <c r="E137" s="53"/>
+      <c r="F137" s="53"/>
+      <c r="G137" s="53"/>
+      <c r="H137" s="53"/>
+      <c r="I137" s="53"/>
+      <c r="J137" s="53"/>
+      <c r="K137" s="53"/>
     </row>
     <row r="138" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F138" s="55" t="s">
+      <c r="F138" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="G138" s="50" t="s">
+      <c r="G138" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="H138" s="51" t="s">
+      <c r="H138" s="38" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="139" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F139" s="45" t="s">
+      <c r="F139" s="32" t="s">
         <v>190</v>
       </c>
       <c r="G139" s="28">
         <v>8</v>
       </c>
-      <c r="H139" s="47">
+      <c r="H139" s="34">
         <v>2</v>
       </c>
     </row>
     <row r="140" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F140" s="56" t="s">
+      <c r="F140" s="43" t="s">
         <v>191</v>
       </c>
-      <c r="G140" s="57">
+      <c r="G140" s="44">
         <v>6</v>
       </c>
-      <c r="H140" s="58">
+      <c r="H140" s="45">
         <v>27</v>
       </c>
     </row>
     <row r="142" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F142" s="32" t="s">
+      <c r="F142" s="52" t="s">
         <v>205</v>
       </c>
-      <c r="G142" s="33"/>
-      <c r="H142" s="33"/>
+      <c r="G142" s="53"/>
+      <c r="H142" s="53"/>
     </row>
     <row r="143" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F143" s="33"/>
-      <c r="G143" s="33"/>
-      <c r="H143" s="33"/>
+      <c r="F143" s="53"/>
+      <c r="G143" s="53"/>
+      <c r="H143" s="53"/>
     </row>
     <row r="144" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F144" s="33"/>
-      <c r="G144" s="33"/>
-      <c r="H144" s="33"/>
+      <c r="F144" s="53"/>
+      <c r="G144" s="53"/>
+      <c r="H144" s="53"/>
     </row>
     <row r="145" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B145" s="33" t="s">
+      <c r="B145" s="53" t="s">
         <v>193</v>
       </c>
-      <c r="C145" s="33"/>
-      <c r="D145" s="33"/>
-      <c r="E145" s="33"/>
-      <c r="F145" s="33"/>
-      <c r="G145" s="33"/>
-      <c r="H145" s="33"/>
-      <c r="I145" s="33"/>
-      <c r="J145" s="33"/>
-      <c r="K145" s="33"/>
+      <c r="C145" s="53"/>
+      <c r="D145" s="53"/>
+      <c r="E145" s="53"/>
+      <c r="F145" s="53"/>
+      <c r="G145" s="53"/>
+      <c r="H145" s="53"/>
+      <c r="I145" s="53"/>
+      <c r="J145" s="53"/>
+      <c r="K145" s="53"/>
     </row>
     <row r="146" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B146" s="33"/>
-      <c r="C146" s="33"/>
-      <c r="D146" s="33"/>
-      <c r="E146" s="33"/>
-      <c r="F146" s="33"/>
-      <c r="G146" s="33"/>
-      <c r="H146" s="33"/>
-      <c r="I146" s="33"/>
-      <c r="J146" s="33"/>
-      <c r="K146" s="33"/>
+      <c r="B146" s="53"/>
+      <c r="C146" s="53"/>
+      <c r="D146" s="53"/>
+      <c r="E146" s="53"/>
+      <c r="F146" s="53"/>
+      <c r="G146" s="53"/>
+      <c r="H146" s="53"/>
+      <c r="I146" s="53"/>
+      <c r="J146" s="53"/>
+      <c r="K146" s="53"/>
     </row>
     <row r="147" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B147" s="33"/>
-      <c r="C147" s="33"/>
-      <c r="D147" s="33"/>
-      <c r="E147" s="33"/>
-      <c r="F147" s="33"/>
-      <c r="G147" s="33"/>
-      <c r="H147" s="33"/>
-      <c r="I147" s="33"/>
-      <c r="J147" s="33"/>
-      <c r="K147" s="33"/>
+      <c r="B147" s="53"/>
+      <c r="C147" s="53"/>
+      <c r="D147" s="53"/>
+      <c r="E147" s="53"/>
+      <c r="F147" s="53"/>
+      <c r="G147" s="53"/>
+      <c r="H147" s="53"/>
+      <c r="I147" s="53"/>
+      <c r="J147" s="53"/>
+      <c r="K147" s="53"/>
     </row>
     <row r="148" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F148" s="55" t="s">
+      <c r="F148" s="42" t="s">
         <v>208</v>
       </c>
-      <c r="G148" s="50" t="s">
+      <c r="G148" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="H148" s="51" t="s">
+      <c r="H148" s="38" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="149" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F149" s="45" t="s">
+      <c r="F149" s="32" t="s">
         <v>190</v>
       </c>
       <c r="G149" s="28">
         <v>2</v>
       </c>
-      <c r="H149" s="47">
+      <c r="H149" s="34">
         <v>8</v>
       </c>
     </row>
     <row r="150" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F150" s="56" t="s">
+      <c r="F150" s="43" t="s">
         <v>191</v>
       </c>
-      <c r="G150" s="57">
+      <c r="G150" s="44">
         <v>12</v>
       </c>
-      <c r="H150" s="58">
+      <c r="H150" s="45">
         <v>21</v>
       </c>
     </row>
     <row r="152" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F152" s="32" t="s">
+      <c r="F152" s="52" t="s">
         <v>206</v>
       </c>
-      <c r="G152" s="33"/>
-      <c r="H152" s="33"/>
+      <c r="G152" s="53"/>
+      <c r="H152" s="53"/>
     </row>
     <row r="153" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F153" s="33"/>
-      <c r="G153" s="33"/>
-      <c r="H153" s="33"/>
+      <c r="F153" s="53"/>
+      <c r="G153" s="53"/>
+      <c r="H153" s="53"/>
     </row>
     <row r="154" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="F154" s="33"/>
-      <c r="G154" s="33"/>
-      <c r="H154" s="33"/>
+      <c r="F154" s="53"/>
+      <c r="G154" s="53"/>
+      <c r="H154" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6958,23 +6605,23 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="255.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="25" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:4" s="25" customFormat="1" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="A1" s="57" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-    </row>
-    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="A2" s="15"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7089,7 +6736,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>117</v>
       </c>
@@ -7243,19 +6890,19 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
@@ -7353,7 +7000,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
         <v>117</v>
       </c>

</xml_diff>